<commit_message>
Ajout numéro TRE type identifiant 8eb6c72ac72d0543b58e45b8c7bc67aa5ecbc38e
</commit_message>
<xml_diff>
--- a/ig/majKereval/StructureDefinition-ror-practitioner.xlsx
+++ b/ig/majKereval/StructureDefinition-ror-practitioner.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="400">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-21T15:32:49+00:00</t>
+    <t>2023-03-27T14:30:28+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -614,7 +614,10 @@
     <t>Practitioner.extension</t>
   </si>
   <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
   </si>
   <si>
     <t>DomainResource.extension</t>
@@ -634,6 +637,22 @@
   </si>
   <si>
     <t>Extension créée dans le cadre du ROR pour définir la civilité de la personne physique</t>
+  </si>
+  <si>
+    <t>Practitioner.extension:ror-meta-creation-date</t>
+  </si>
+  <si>
+    <t>ror-meta-creation-date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/ror30/StructureDefinition/ror-meta-creation-date}
+</t>
+  </si>
+  <si>
+    <t>dateCreation (Metadonnee)</t>
+  </si>
+  <si>
+    <t>Extension créée dans le cadre du ROR qui correspond à la date de création (dans le ROR régionnal) présente dans les métadonnées.</t>
   </si>
   <si>
     <t>Practitioner.modifierExtension</t>
@@ -783,12 +802,6 @@
   </si>
   <si>
     <t>2</t>
-  </si>
-  <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>An Extension</t>
   </si>
   <si>
     <t>Practitioner.telecom.extension:ror-telecom-communication-channel</t>
@@ -1549,7 +1562,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN47"/>
+  <dimension ref="A1:AN48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2412,7 +2425,7 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G8" t="s" s="2">
         <v>84</v>
@@ -3548,11 +3561,11 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>76</v>
@@ -3570,14 +3583,12 @@
         <v>107</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>108</v>
+        <v>193</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="N18" t="s" s="2">
-        <v>110</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
         <v>74</v>
@@ -3626,7 +3637,7 @@
         <v>113</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>75</v>
@@ -3644,7 +3655,7 @@
         <v>74</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="AM18" t="s" s="2">
         <v>74</v>
@@ -3655,13 +3666,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B19" t="s" s="2">
         <v>192</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D19" t="s" s="2">
         <v>74</v>
@@ -3683,13 +3694,13 @@
         <v>74</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -3740,7 +3751,7 @@
         <v>74</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>75</v>
@@ -3769,46 +3780,44 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>192</v>
+      </c>
+      <c r="C20" t="s" s="2">
+        <v>202</v>
+      </c>
       <c r="D20" t="s" s="2">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>74</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="J20" t="s" s="2">
         <v>74</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>107</v>
+        <v>203</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="O20" t="s" s="2">
-        <v>203</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
       <c r="P20" t="s" s="2">
         <v>74</v>
       </c>
@@ -3844,19 +3853,19 @@
         <v>74</v>
       </c>
       <c r="AB20" t="s" s="2">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="AC20" t="s" s="2">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="AD20" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>75</v>
@@ -3874,7 +3883,7 @@
         <v>74</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="AM20" t="s" s="2">
         <v>74</v>
@@ -3885,33 +3894,33 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>74</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>206</v>
+        <v>107</v>
       </c>
       <c r="L21" t="s" s="2">
         <v>207</v>
@@ -3919,7 +3928,9 @@
       <c r="M21" t="s" s="2">
         <v>208</v>
       </c>
-      <c r="N21" s="2"/>
+      <c r="N21" t="s" s="2">
+        <v>110</v>
+      </c>
       <c r="O21" t="s" s="2">
         <v>209</v>
       </c>
@@ -3958,19 +3969,19 @@
         <v>74</v>
       </c>
       <c r="AB21" t="s" s="2">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="AC21" t="s" s="2">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="AD21" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>75</v>
@@ -3982,27 +3993,27 @@
         <v>96</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>210</v>
+        <v>74</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>211</v>
+        <v>98</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>212</v>
+        <v>74</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>213</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4010,7 +4021,7 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>84</v>
@@ -4025,26 +4036,22 @@
         <v>85</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="L22" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="N22" s="2"/>
+      <c r="O22" t="s" s="2">
         <v>215</v>
       </c>
-      <c r="L22" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="O22" t="s" s="2">
-        <v>219</v>
-      </c>
       <c r="P22" t="s" s="2">
         <v>74</v>
       </c>
-      <c r="Q22" t="s" s="2">
-        <v>220</v>
-      </c>
+      <c r="Q22" s="2"/>
       <c r="R22" t="s" s="2">
         <v>74</v>
       </c>
@@ -4088,13 +4095,13 @@
         <v>74</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>96</v>
@@ -4103,24 +4110,24 @@
         <v>97</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>74</v>
+        <v>216</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>74</v>
+        <v>218</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4131,7 +4138,7 @@
         <v>75</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>74</v>
@@ -4143,24 +4150,26 @@
         <v>85</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="L23" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="N23" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="O23" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="M23" t="s" s="2">
+      <c r="P23" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q23" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="N23" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="O23" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="P23" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Q23" s="2"/>
       <c r="R23" t="s" s="2">
         <v>74</v>
       </c>
@@ -4204,13 +4213,13 @@
         <v>74</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>96</v>
@@ -4219,24 +4228,24 @@
         <v>97</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>229</v>
+        <v>74</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>231</v>
+        <v>74</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>74</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4259,19 +4268,19 @@
         <v>85</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L24" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="M24" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="N24" t="s" s="2">
         <v>233</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="O24" t="s" s="2">
         <v>234</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="O24" t="s" s="2">
-        <v>237</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>74</v>
@@ -4320,7 +4329,7 @@
         <v>74</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>75</v>
@@ -4332,16 +4341,16 @@
         <v>96</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>238</v>
+        <v>97</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>74</v>
@@ -4349,10 +4358,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4363,7 +4372,7 @@
         <v>75</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>74</v>
@@ -4372,19 +4381,23 @@
         <v>74</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>100</v>
+        <v>239</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>101</v>
+        <v>240</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
+        <v>241</v>
+      </c>
+      <c r="N25" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="O25" t="s" s="2">
+        <v>243</v>
+      </c>
       <c r="P25" t="s" s="2">
         <v>74</v>
       </c>
@@ -4432,28 +4445,28 @@
         <v>74</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>103</v>
+        <v>238</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>74</v>
+        <v>244</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>74</v>
+        <v>245</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>104</v>
+        <v>246</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>74</v>
+        <v>247</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>74</v>
@@ -4461,10 +4474,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4472,10 +4485,10 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
-        <v>244</v>
+        <v>75</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>74</v>
@@ -4487,13 +4500,13 @@
         <v>74</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>245</v>
+        <v>101</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>246</v>
+        <v>102</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -4532,37 +4545,37 @@
         <v>74</v>
       </c>
       <c r="AB26" t="s" s="2">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="AC26" t="s" s="2">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="AD26" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>74</v>
@@ -4573,23 +4586,21 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="C27" t="s" s="2">
-        <v>248</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
         <v>74</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s" s="2">
-        <v>84</v>
+        <v>250</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>74</v>
@@ -4601,13 +4612,13 @@
         <v>74</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>249</v>
+        <v>107</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>250</v>
+        <v>193</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>251</v>
+        <v>194</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -4646,16 +4657,16 @@
         <v>74</v>
       </c>
       <c r="AB27" t="s" s="2">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="AC27" t="s" s="2">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="AD27" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>114</v>
@@ -4687,20 +4698,20 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="B28" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="C28" t="s" s="2">
         <v>252</v>
-      </c>
-      <c r="B28" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="C28" t="s" s="2">
-        <v>253</v>
       </c>
       <c r="D28" t="s" s="2">
         <v>74</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>84</v>
@@ -4715,13 +4726,13 @@
         <v>74</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>254</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>255</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>256</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -4801,20 +4812,20 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="C29" t="s" s="2">
         <v>257</v>
-      </c>
-      <c r="B29" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="C29" t="s" s="2">
-        <v>258</v>
       </c>
       <c r="D29" t="s" s="2">
         <v>74</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>84</v>
@@ -4829,13 +4840,13 @@
         <v>74</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>260</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>261</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -4915,18 +4926,20 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="B30" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="C30" t="s" s="2">
         <v>262</v>
       </c>
-      <c r="B30" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
         <v>74</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>84</v>
@@ -4938,20 +4951,18 @@
         <v>74</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>169</v>
+        <v>263</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="N30" t="s" s="2">
         <v>265</v>
       </c>
+      <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
         <v>74</v>
@@ -4976,13 +4987,13 @@
         <v>74</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>266</v>
+        <v>74</v>
       </c>
       <c r="Z30" t="s" s="2">
-        <v>267</v>
+        <v>74</v>
       </c>
       <c r="AA30" t="s" s="2">
         <v>74</v>
@@ -5000,28 +5011,28 @@
         <v>74</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>268</v>
+        <v>114</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>269</v>
+        <v>96</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>270</v>
+        <v>74</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>271</v>
+        <v>74</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>272</v>
+        <v>74</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>74</v>
@@ -5029,10 +5040,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5040,7 +5051,7 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>84</v>
@@ -5055,20 +5066,18 @@
         <v>85</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="O31" t="s" s="2">
-        <v>277</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
         <v>74</v>
       </c>
@@ -5092,13 +5101,13 @@
         <v>74</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>74</v>
+        <v>270</v>
       </c>
       <c r="Z31" t="s" s="2">
-        <v>74</v>
+        <v>271</v>
       </c>
       <c r="AA31" t="s" s="2">
         <v>74</v>
@@ -5116,7 +5125,7 @@
         <v>74</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>75</v>
@@ -5125,19 +5134,19 @@
         <v>84</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>96</v>
+        <v>273</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>97</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>74</v>
@@ -5145,10 +5154,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5156,7 +5165,7 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>84</v>
@@ -5165,25 +5174,25 @@
         <v>74</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="J32" t="s" s="2">
         <v>85</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>169</v>
+        <v>100</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="O32" t="s" s="2">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>74</v>
@@ -5208,13 +5217,13 @@
         <v>74</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>287</v>
+        <v>74</v>
       </c>
       <c r="Z32" t="s" s="2">
-        <v>288</v>
+        <v>74</v>
       </c>
       <c r="AA32" t="s" s="2">
         <v>74</v>
@@ -5232,7 +5241,7 @@
         <v>74</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>75</v>
@@ -5247,13 +5256,13 @@
         <v>97</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>74</v>
@@ -5261,10 +5270,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5281,24 +5290,26 @@
         <v>74</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="J33" t="s" s="2">
         <v>85</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>294</v>
+        <v>169</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="O33" s="2"/>
+        <v>289</v>
+      </c>
+      <c r="O33" t="s" s="2">
+        <v>290</v>
+      </c>
       <c r="P33" t="s" s="2">
         <v>74</v>
       </c>
@@ -5322,13 +5333,13 @@
         <v>74</v>
       </c>
       <c r="X33" t="s" s="2">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>74</v>
+        <v>291</v>
       </c>
       <c r="Z33" t="s" s="2">
-        <v>74</v>
+        <v>292</v>
       </c>
       <c r="AA33" t="s" s="2">
         <v>74</v>
@@ -5346,7 +5357,7 @@
         <v>74</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>75</v>
@@ -5361,13 +5372,13 @@
         <v>97</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>104</v>
+        <v>294</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>104</v>
+        <v>295</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>74</v>
+        <v>296</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>74</v>
@@ -5375,10 +5386,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5401,16 +5412,16 @@
         <v>85</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="L34" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="M34" t="s" s="2">
         <v>300</v>
       </c>
-      <c r="L34" t="s" s="2">
+      <c r="N34" t="s" s="2">
         <v>301</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
@@ -5460,7 +5471,7 @@
         <v>74</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>75</v>
@@ -5472,16 +5483,16 @@
         <v>96</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>305</v>
+        <v>97</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>306</v>
+        <v>104</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>307</v>
+        <v>74</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>74</v>
@@ -5489,10 +5500,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5503,7 +5514,7 @@
         <v>75</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>74</v>
@@ -5515,20 +5526,18 @@
         <v>85</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="O35" t="s" s="2">
-        <v>313</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
         <v>74</v>
       </c>
@@ -5582,22 +5591,22 @@
         <v>75</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>96</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>97</v>
+        <v>309</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>314</v>
+        <v>98</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>74</v>
@@ -5605,10 +5614,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5619,7 +5628,7 @@
         <v>75</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>74</v>
@@ -5631,19 +5640,19 @@
         <v>85</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>169</v>
+        <v>313</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>265</v>
+        <v>316</v>
       </c>
       <c r="O36" t="s" s="2">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>74</v>
@@ -5668,13 +5677,13 @@
         <v>74</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>321</v>
+        <v>74</v>
       </c>
       <c r="Z36" t="s" s="2">
-        <v>322</v>
+        <v>74</v>
       </c>
       <c r="AA36" t="s" s="2">
         <v>74</v>
@@ -5692,13 +5701,13 @@
         <v>74</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>96</v>
@@ -5707,13 +5716,13 @@
         <v>97</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>74</v>
@@ -5721,10 +5730,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5747,17 +5756,19 @@
         <v>85</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>327</v>
+        <v>169</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="N37" s="2"/>
+        <v>323</v>
+      </c>
+      <c r="N37" t="s" s="2">
+        <v>269</v>
+      </c>
       <c r="O37" t="s" s="2">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>74</v>
@@ -5782,13 +5793,13 @@
         <v>74</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>74</v>
+        <v>325</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>74</v>
+        <v>326</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>74</v>
@@ -5806,7 +5817,7 @@
         <v>74</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>75</v>
@@ -5821,13 +5832,13 @@
         <v>97</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>74</v>
@@ -5835,10 +5846,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5849,7 +5860,7 @@
         <v>75</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>74</v>
@@ -5858,22 +5869,20 @@
         <v>74</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>338</v>
-      </c>
+        <v>333</v>
+      </c>
+      <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>74</v>
@@ -5922,28 +5931,28 @@
         <v>74</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>96</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>340</v>
+        <v>97</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>74</v>
@@ -5951,10 +5960,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -5977,16 +5986,20 @@
         <v>74</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
+        <v>341</v>
+      </c>
+      <c r="N39" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="O39" t="s" s="2">
+        <v>343</v>
+      </c>
       <c r="P39" t="s" s="2">
         <v>74</v>
       </c>
@@ -6034,7 +6047,7 @@
         <v>74</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>75</v>
@@ -6046,16 +6059,16 @@
         <v>96</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>97</v>
+        <v>344</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>74</v>
@@ -6063,10 +6076,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6077,7 +6090,7 @@
         <v>75</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>74</v>
@@ -6089,13 +6102,13 @@
         <v>74</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>100</v>
+        <v>349</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>101</v>
+        <v>350</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>102</v>
+        <v>351</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6146,28 +6159,28 @@
         <v>74</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>103</v>
+        <v>348</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>74</v>
+        <v>352</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>104</v>
+        <v>353</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>74</v>
+        <v>354</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>74</v>
@@ -6175,21 +6188,21 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
         <v>75</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>74</v>
@@ -6201,17 +6214,15 @@
         <v>74</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>110</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="N41" s="2"/>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
         <v>74</v>
@@ -6248,37 +6259,37 @@
         <v>74</v>
       </c>
       <c r="AB41" t="s" s="2">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="AC41" t="s" s="2">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="AD41" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH41" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>74</v>
@@ -6289,14 +6300,14 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
-        <v>354</v>
+        <v>106</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
@@ -6309,26 +6320,24 @@
         <v>74</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K42" t="s" s="2">
         <v>107</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>355</v>
+        <v>108</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>356</v>
+        <v>109</v>
       </c>
       <c r="N42" t="s" s="2">
         <v>110</v>
       </c>
-      <c r="O42" t="s" s="2">
-        <v>203</v>
-      </c>
+      <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
         <v>74</v>
       </c>
@@ -6364,19 +6373,19 @@
         <v>74</v>
       </c>
       <c r="AB42" t="s" s="2">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="AC42" t="s" s="2">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="AD42" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>357</v>
+        <v>114</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>75</v>
@@ -6405,14 +6414,14 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
-        <v>74</v>
+        <v>358</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s" s="2">
@@ -6425,13 +6434,13 @@
         <v>74</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>206</v>
+        <v>107</v>
       </c>
       <c r="L43" t="s" s="2">
         <v>359</v>
@@ -6439,9 +6448,11 @@
       <c r="M43" t="s" s="2">
         <v>360</v>
       </c>
-      <c r="N43" s="2"/>
+      <c r="N43" t="s" s="2">
+        <v>110</v>
+      </c>
       <c r="O43" t="s" s="2">
-        <v>361</v>
+        <v>209</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>74</v>
@@ -6490,7 +6501,7 @@
         <v>74</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>75</v>
@@ -6502,16 +6513,16 @@
         <v>96</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>362</v>
+        <v>74</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>363</v>
+        <v>98</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>364</v>
+        <v>74</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>74</v>
@@ -6519,10 +6530,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6530,10 +6541,10 @@
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>74</v>
@@ -6545,18 +6556,18 @@
         <v>74</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>366</v>
+        <v>212</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="O44" s="2"/>
+        <v>364</v>
+      </c>
+      <c r="N44" s="2"/>
+      <c r="O44" t="s" s="2">
+        <v>365</v>
+      </c>
       <c r="P44" t="s" s="2">
         <v>74</v>
       </c>
@@ -6580,13 +6591,13 @@
         <v>74</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>154</v>
+        <v>74</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>370</v>
+        <v>74</v>
       </c>
       <c r="Z44" t="s" s="2">
-        <v>371</v>
+        <v>74</v>
       </c>
       <c r="AA44" t="s" s="2">
         <v>74</v>
@@ -6604,13 +6615,13 @@
         <v>74</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI44" t="s" s="2">
         <v>96</v>
@@ -6619,13 +6630,13 @@
         <v>97</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>349</v>
+        <v>367</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>74</v>
@@ -6633,10 +6644,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6644,7 +6655,7 @@
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>84</v>
@@ -6659,20 +6670,18 @@
         <v>74</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>300</v>
+        <v>370</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="O45" t="s" s="2">
-        <v>377</v>
-      </c>
+        <v>373</v>
+      </c>
+      <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
         <v>74</v>
       </c>
@@ -6696,13 +6705,13 @@
         <v>74</v>
       </c>
       <c r="X45" t="s" s="2">
-        <v>74</v>
+        <v>154</v>
       </c>
       <c r="Y45" t="s" s="2">
-        <v>74</v>
+        <v>374</v>
       </c>
       <c r="Z45" t="s" s="2">
-        <v>74</v>
+        <v>375</v>
       </c>
       <c r="AA45" t="s" s="2">
         <v>74</v>
@@ -6720,10 +6729,10 @@
         <v>74</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>84</v>
@@ -6732,16 +6741,16 @@
         <v>96</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>305</v>
+        <v>97</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>379</v>
+        <v>353</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>74</v>
@@ -6749,10 +6758,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6775,18 +6784,20 @@
         <v>74</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>382</v>
+        <v>304</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>385</v>
-      </c>
-      <c r="O46" s="2"/>
+        <v>307</v>
+      </c>
+      <c r="O46" t="s" s="2">
+        <v>381</v>
+      </c>
       <c r="P46" t="s" s="2">
         <v>74</v>
       </c>
@@ -6834,7 +6845,7 @@
         <v>74</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>75</v>
@@ -6846,16 +6857,16 @@
         <v>96</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>386</v>
+        <v>309</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>74</v>
+        <v>382</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>74</v>
+        <v>384</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>74</v>
@@ -6863,10 +6874,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -6877,7 +6888,7 @@
         <v>75</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H47" t="s" s="2">
         <v>74</v>
@@ -6889,20 +6900,18 @@
         <v>74</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>366</v>
+        <v>386</v>
       </c>
       <c r="L47" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="N47" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="M47" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>391</v>
-      </c>
-      <c r="O47" t="s" s="2">
-        <v>392</v>
-      </c>
+      <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
         <v>74</v>
       </c>
@@ -6926,13 +6935,13 @@
         <v>74</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>173</v>
+        <v>74</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>174</v>
+        <v>74</v>
       </c>
       <c r="Z47" t="s" s="2">
-        <v>175</v>
+        <v>74</v>
       </c>
       <c r="AA47" t="s" s="2">
         <v>74</v>
@@ -6950,30 +6959,146 @@
         <v>74</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI47" t="s" s="2">
         <v>96</v>
       </c>
       <c r="AJ47" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL47" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="AM47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AN47" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="B48" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G48" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="K48" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="L48" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="O48" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="P48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q48" s="2"/>
+      <c r="R48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X48" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="Y48" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="Z48" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="AA48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF48" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="AG48" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH48" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI48" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AJ48" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="AK47" t="s" s="2">
-        <v>393</v>
-      </c>
-      <c r="AL47" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="AM47" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="AN47" t="s" s="2">
+      <c r="AK48" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="AL48" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="AM48" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="AN48" t="s" s="2">
         <v>74</v>
       </c>
     </row>

</xml_diff>